<commit_message>
rm mmg/parmmg from benchmarking, it will be indirectly benchmarked
</commit_message>
<xml_diff>
--- a/exama-software.xlsx
+++ b/exama-software.xlsx
@@ -98,7 +98,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2222" uniqueCount="1143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2220" uniqueCount="1143">
   <si>
     <t>Software</t>
   </si>
@@ -7969,7 +7969,7 @@
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Benchmarks" cacheId="0" dataCaption="" rowGrandTotals="0" compact="0" compactData="0">
-  <location ref="A1:K14" firstHeaderRow="0" firstDataRow="10" firstDataCol="0"/>
+  <location ref="A1:K13" firstHeaderRow="0" firstDataRow="10" firstDataCol="0"/>
   <pivotFields>
     <pivotField name="Software" axis="axisRow" compact="0" outline="0" multipleItemSelectionAllowed="1" showAll="0" sortType="ascending" defaultSubtotal="0">
       <items>
@@ -18224,7 +18224,7 @@
       <c r="D23" s="19"/>
       <c r="E23" s="19"/>
       <c r="F23" s="5" t="s">
-        <v>65</v>
+        <v>114</v>
       </c>
       <c r="G23" s="10"/>
       <c r="H23" s="10"/>
@@ -18253,7 +18253,7 @@
         <v>225</v>
       </c>
       <c r="S23" s="4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T23" s="10"/>
       <c r="U23" s="10" t="b">
@@ -42985,7 +42985,10 @@
     <row r="11"/>
     <row r="12"/>
     <row r="13"/>
-    <row r="14"/>
+    <row r="14">
+      <c r="B14" s="36"/>
+      <c r="D14" s="37"/>
+    </row>
     <row r="15">
       <c r="B15" s="36"/>
       <c r="D15" s="37"/>

</xml_diff>

<commit_message>
minor fixes thanks @prj-
- use cleverref
- Bemchmarked->benchmarked
- PaStIX -> PaStiX @lgiraud-Inria

- mmg/parmmg is now indirectly benchmarked
</commit_message>
<xml_diff>
--- a/exama-software.xlsx
+++ b/exama-software.xlsx
@@ -378,7 +378,7 @@
 krylov solver</t>
   </si>
   <si>
-    <t>PaStIX,
+    <t>PaStiX,
 qr_mumps,
 MUMPS,
 Scotch</t>
@@ -777,7 +777,7 @@
 Feel++,
 PETSc,
 MUMPS,
-PaStIX</t>
+PaStiX</t>
   </si>
   <si>
     <t>ICoCo coupling interface</t>
@@ -961,7 +961,7 @@
 Test - Validation</t>
   </si>
   <si>
-    <t>PaStIX</t>
+    <t>PaStiX</t>
   </si>
   <si>
     <t>Inria, Université Bordeaux, BINP</t>
@@ -1059,8 +1059,7 @@
 MMG/ParMMG,
 MUMPS,
 Scotch,
-PaStIX,
-HPdomain decomposition methods</t>
+PaStiX, HPDDM</t>
   </si>
   <si>
     <t>PLEIADES</t>
@@ -6557,7 +6556,7 @@
         <s v="MMG/ParMMG"/>
         <s v="MUMPS"/>
         <s v="OpenTURNS"/>
-        <s v="PaStIX"/>
+        <s v="PaStiX"/>
         <s v="pBB"/>
         <s v="PETSc"/>
         <s v="PLEIADES"/>
@@ -7033,7 +7032,7 @@
         <s v="MMG/ParMMG"/>
         <s v="MUMPS"/>
         <s v="OpenTURNS"/>
-        <s v="PaStIX"/>
+        <s v="PaStiX"/>
         <s v="pBB"/>
         <s v="PETSc"/>
         <s v="PLEIADES"/>
@@ -7451,14 +7450,14 @@
     <cacheField name="Interfaces" numFmtId="0">
       <sharedItems containsBlank="1">
         <m/>
-        <s v="PaStIX,&#10;qr_mumps,&#10;MUMPS,&#10;Scotch"/>
+        <s v="PaStiX,&#10;qr_mumps,&#10;MUMPS,&#10;Scotch"/>
         <s v="OpenTurns,&#10;MMG/ParMMG,&#10;PETSc,&#10;Salome,&#10;Dymola/OpenModelica/FMU,&#10;HPdomain decomposition methods"/>
         <s v="PETSc,&#10;MMG/ParMMG,&#10;Scotch,&#10;MUMPS,&#10;HPdomain decomposition methods"/>
         <s v="MUMPS"/>
-        <s v="Freefem++,&#10;Feel++,&#10;PETSc,&#10;MUMPS,&#10;PaStIX"/>
+        <s v="Freefem++,&#10;Feel++,&#10;PETSc,&#10;MUMPS,&#10;PaStiX"/>
         <s v="Arcane Framework"/>
         <s v="Scotch"/>
-        <s v="Freefem++,&#10;Feel++,&#10;MMG/ParMMG,&#10;MUMPS,&#10;Scotch,&#10;PaStIX,&#10;HPdomain decomposition methods"/>
+        <s v="Freefem++,&#10;Feel++,&#10;MMG/ParMMG,&#10;MUMPS,&#10;Scotch,&#10;PaStiX, HPDDM"/>
         <s v="CADNA"/>
         <s v="StarPU,&#10;Scotch"/>
         <s v="PETSc"/>
@@ -7503,7 +7502,7 @@
         <s v="MMG/ParMMG"/>
         <s v="MUMPS"/>
         <s v="OpenTURNS"/>
-        <s v="PaStIX"/>
+        <s v="PaStiX"/>
         <s v="pBB"/>
         <s v="PETSc"/>
         <s v="PLEIADES"/>
@@ -7946,14 +7945,14 @@
     <cacheField name="Interfaces" numFmtId="0">
       <sharedItems containsBlank="1">
         <m/>
-        <s v="PaStIX,&#10;qr_mumps,&#10;MUMPS,&#10;Scotch"/>
+        <s v="PaStiX,&#10;qr_mumps,&#10;MUMPS,&#10;Scotch"/>
         <s v="OpenTurns,&#10;MMG/ParMMG,&#10;PETSc,&#10;Salome,&#10;Dymola/OpenModelica/FMU,&#10;HPdomain decomposition methods"/>
         <s v="PETSc,&#10;MMG/ParMMG,&#10;Scotch,&#10;MUMPS,&#10;HPdomain decomposition methods"/>
         <s v="MUMPS"/>
-        <s v="Freefem++,&#10;Feel++,&#10;PETSc,&#10;MUMPS,&#10;PaStIX"/>
+        <s v="Freefem++,&#10;Feel++,&#10;PETSc,&#10;MUMPS,&#10;PaStiX"/>
         <s v="Arcane Framework"/>
         <s v="Scotch"/>
-        <s v="Freefem++,&#10;Feel++,&#10;MMG/ParMMG,&#10;MUMPS,&#10;Scotch,&#10;PaStIX,&#10;HPdomain decomposition methods"/>
+        <s v="Freefem++,&#10;Feel++,&#10;MMG/ParMMG,&#10;MUMPS,&#10;Scotch,&#10;PaStiX, HPDDM"/>
         <s v="CADNA"/>
         <s v="StarPU,&#10;Scotch"/>
         <s v="PETSc"/>

</xml_diff>

<commit_message>
added @clgch in the list of contributors for Uranie
/cc @rchocat
</commit_message>
<xml_diff>
--- a/exama-software.xlsx
+++ b/exama-software.xlsx
@@ -1300,7 +1300,7 @@
     <t>Uranie</t>
   </si>
   <si>
-    <t>rudy.chocat@cea.fr, jean-baptiste.blanchard@cea.fr</t>
+    <t>rudy.chocat@cea.fr, jean-baptiste.blanchard@cea.fr,clement.gauchy@cea.fr</t>
   </si>
   <si>
     <t>https://sourceforge.net/projects/uranie/</t>
@@ -6599,7 +6599,7 @@
         <s v="emmanuel.franck@inria.fr"/>
         <s v="berenger.bramas@inria.fr"/>
         <s v="pierre.ledac@cea.fr"/>
-        <s v="rudy.chocat@cea.fr, jean-baptiste.blanchard@cea.fr"/>
+        <s v="rudy.chocat@cea.fr, jean-baptiste.blanchard@cea.fr,clement.gauchy@cea.fr"/>
         <s v="el-ghazali.talbi@univ-lille.fr"/>
       </sharedItems>
     </cacheField>
@@ -7545,7 +7545,7 @@
         <s v="emmanuel.franck@inria.fr"/>
         <s v="berenger.bramas@inria.fr"/>
         <s v="pierre.ledac@cea.fr"/>
-        <s v="rudy.chocat@cea.fr, jean-baptiste.blanchard@cea.fr"/>
+        <s v="rudy.chocat@cea.fr, jean-baptiste.blanchard@cea.fr,clement.gauchy@cea.fr"/>
         <s v="el-ghazali.talbi@univ-lille.fr"/>
       </sharedItems>
     </cacheField>

</xml_diff>